<commit_message>
20200916 INT20-0030	Fix to reload JS file for TimeoutReminder 20200923 CRE20-007-02	Launch of 2020_21 VSS, RVP and School Outreach Vaccination – Phase 2 20200923 CRE20-008	To have search Function for Non-Clinic Setting at SDIR 20200923 CRS20-016	Update of Enrolment Application Form (Appendix A) of Vaccination Subsidy Scheme (VSS), Residential Care Home Vaccination Programme (RVP) and Health Care Voucher Scheme (HCVS) 20200929 CRE17-004	To generate a new DPAR on EHCP basis for monthly reimbursement exercise 20200929 INT20-0032	Fix new add account in VU Vacc File Rectification
</commit_message>
<xml_diff>
--- a/EHS2019/EHS/ExcelGenerator/Template/eHSM0001-PreAuthorizationRMB_Template.xlsx
+++ b/EHS2019/EHS/ExcelGenerator/Template/eHSM0001-PreAuthorizationRMB_Template.xlsx
@@ -1,24 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN\trunk\EHS2019\EHS\ExcelGenerator\bin\Debug\Template\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="2700" yWindow="60" windowWidth="15660" windowHeight="9675"/>
   </bookViews>
   <sheets>
     <sheet name="Content" sheetId="1" r:id="rId1"/>
     <sheet name="Summary" sheetId="2" r:id="rId2"/>
-    <sheet name="01" sheetId="3" r:id="rId3"/>
-    <sheet name="Remark" sheetId="4" r:id="rId4"/>
-    <sheet name="Change History" sheetId="5" r:id="rId5"/>
+    <sheet name="01" sheetId="7" r:id="rId3"/>
+    <sheet name="02" sheetId="6" r:id="rId4"/>
+    <sheet name="03" sheetId="3" r:id="rId5"/>
+    <sheet name="Remark" sheetId="4" r:id="rId6"/>
+    <sheet name="Change History" sheetId="5" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="74">
   <si>
     <t>Residential Care Home Seasonal Influenza Vaccination for Health Care Worker</t>
   </si>
@@ -108,10 +115,6 @@
   <si>
     <t>Sub Report Name</t>
     <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pre Authorization Checking File</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>2. Subsidy Legend</t>
@@ -275,13 +278,32 @@
     <t>计划代码</t>
   </si>
   <si>
+    <t>CRE15-006</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rename of eHS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>eHS(S)M0001-01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">eHS(S)M0001-01: </t>
-    </r>
+  </si>
+  <si>
+    <t>eHS(S)M0001-02</t>
+  </si>
+  <si>
+    <t>eHS(S)M0001-03</t>
+  </si>
+  <si>
+    <t>号码</t>
+  </si>
+  <si>
+    <t>服务提供者号码</t>
+  </si>
+  <si>
+    <t>交易数目</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -290,23 +312,138 @@
         <family val="3"/>
         <charset val="136"/>
       </rPr>
-      <t>授权付款前查核文件</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>CRE15-006</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rename of eHS</t>
+      <t>申报的医疗券金额</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> ($)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>申报的医疗券金额</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (¥)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>申报的医疗券金额</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> ($)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>申报的医疗券金额</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (¥)</t>
+    </r>
+  </si>
+  <si>
+    <t>CRE17-004</t>
+  </si>
+  <si>
+    <t>To generate a new Detailed Payment Analysis Report (DPAR) on EHCP basis for monthly reimbursement exercise</t>
+  </si>
+  <si>
+    <t>Pre Authorization Checking File (on EHCP Basis)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pre Authorization Checking File (on Practice Basis)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pre Authorization Checking File (on Transaction Basis)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">eHS(S)M0001-01: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>授权付款前查核文件(按服务提供者分类)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">eHS(S)M0001-02: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>授权付款前查核文件(按执业处所分类)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">eHS(S)M0001-03: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>授权付款前查核文件(按交易分类)</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="7">
     <numFmt numFmtId="176" formatCode="d\ mmm\ yyyy\ h:mm"/>
     <numFmt numFmtId="177" formatCode="yyyy/mm/dd"/>
@@ -384,7 +521,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -474,6 +611,12 @@
     </xf>
     <xf numFmtId="182" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -485,6 +628,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -533,7 +679,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -568,7 +714,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -777,7 +923,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -795,15 +941,39 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>29</v>
+      <c r="A2" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -824,7 +994,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="16.375" style="12" customWidth="1"/>
+    <col min="2" max="2" width="18.625" style="12" customWidth="1"/>
     <col min="3" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
@@ -878,6 +1048,145 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.375" style="12" customWidth="1"/>
+    <col min="2" max="2" width="16.5" style="6" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="6" customWidth="1"/>
+    <col min="4" max="4" width="16.75" style="6" customWidth="1"/>
+    <col min="5" max="5" width="11.625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="11.625" style="20" customWidth="1"/>
+    <col min="7" max="7" width="16.625" style="6" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="27" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+    </row>
+    <row r="4" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5" style="6" customWidth="1"/>
+    <col min="2" max="2" width="25.5" style="19" customWidth="1"/>
+    <col min="3" max="3" width="25.125" style="19" customWidth="1"/>
+    <col min="4" max="4" width="21.375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="20.625" style="23" customWidth="1"/>
+    <col min="6" max="6" width="11.625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="11.625" style="21" customWidth="1"/>
+    <col min="8" max="8" width="16.625" style="6" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="27" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+    </row>
+    <row r="4" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
@@ -901,7 +1210,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
@@ -914,50 +1223,41 @@
     </row>
     <row r="3" spans="1:14" s="27" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="C3" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="D3" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="E3" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="F3" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="G3" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="H3" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="I3" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="I3" s="25" t="s">
+      <c r="K3" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="J3" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="K3" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="L3" s="24" t="str">
-        <f>IF(LEN(L4) &gt; 0,"Subsidy","")</f>
-        <v/>
-      </c>
-      <c r="M3" s="24" t="str">
-        <f>IF(LEN(M4) &gt; 0,"RCH Code","")</f>
-        <v/>
-      </c>
-      <c r="N3" s="24" t="str">
-        <f>IF(LEN(N4) &gt; 0,"RCH Type", "")</f>
-        <v/>
-      </c>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
     </row>
     <row r="4" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
@@ -983,7 +1283,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -997,7 +1297,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>24</v>
@@ -1005,7 +1305,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1050,7 +1350,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1117,9 +1417,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1134,21 +1434,21 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1156,10 +1456,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="D4" s="10">
         <v>41679</v>
@@ -1170,10 +1470,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="D5" s="10">
         <v>41821</v>
@@ -1184,10 +1484,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>42</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>43</v>
       </c>
       <c r="D6" s="10">
         <v>42213</v>
@@ -1198,13 +1498,27 @@
         <v>4</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D7" s="10">
         <v>42430</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="19">
+        <v>5</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="10">
+        <v>44103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>